<commit_message>
Fix template cell properties
</commit_message>
<xml_diff>
--- a/src/main/resources/template/OssCheckList.xlsx
+++ b/src/main/resources/template/OssCheckList.xlsx
@@ -1716,6 +1716,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="33" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1733,24 +1751,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="33" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -2123,19 +2123,19 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
   <cols>
     <col min="1" max="1" width="37.3984375" customWidth="1"/>
-    <col min="2" max="2" width="45.69921875" style="32" customWidth="1"/>
-    <col min="3" max="3" width="120.59765625" style="33" customWidth="1"/>
+    <col min="2" max="2" width="45.69921875" style="26" customWidth="1"/>
+    <col min="3" max="3" width="120.59765625" style="27" customWidth="1"/>
     <col min="5" max="5" width="20.09765625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="25" t="s">
         <v>236</v>
       </c>
     </row>
@@ -2143,13 +2143,13 @@
       <c r="A2" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="B2" s="34"/>
+      <c r="B2" s="28"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="B3" s="34"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="13" t="s">
         <v>233</v>
       </c>
@@ -2158,13 +2158,13 @@
       <c r="A4" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="B4" s="35"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="13" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="25" t="s">
         <v>237</v>
       </c>
     </row>
@@ -2172,7 +2172,7 @@
       <c r="A7" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="B7" s="34"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="13" t="s">
         <v>245</v>
       </c>
@@ -2181,7 +2181,7 @@
       <c r="A8" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="B8" s="36"/>
+      <c r="B8" s="30"/>
       <c r="C8" s="13" t="s">
         <v>243</v>
       </c>
@@ -2190,7 +2190,7 @@
       <c r="A9" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="B9" s="34"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="13" t="s">
         <v>244</v>
       </c>
@@ -2199,7 +2199,7 @@
       <c r="A10" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="B10" s="34"/>
+      <c r="B10" s="30"/>
       <c r="C10" s="13" t="s">
         <v>246</v>
       </c>
@@ -2208,14 +2208,11 @@
       <c r="A11" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="B11" s="34"/>
+      <c r="B11" s="30"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B11">
-      <formula1>"Yes, No"</formula1>
-    </dataValidation>
+  <dataValidations count="1">
     <dataValidation allowBlank="1" showInputMessage="1" sqref="B3"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2223,24 +2220,6 @@
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri"&amp;12&amp;K000000LGE Internal Use Only&amp;1#</oddHeader>
   </headerFooter>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
-          <x14:formula1>
-            <xm:f>'[1].Data'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B9</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
-          <x14:formula1>
-            <xm:f>'[1].Data'!#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>B10</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -26732,22 +26711,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="31" t="s">
         <v>204</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="4" t="s">
@@ -34281,52 +34260,52 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="33" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="30"/>
-      <c r="F2" s="30"/>
-      <c r="G2" s="30"/>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
     </row>
     <row r="3" spans="1:11">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="33" t="s">
         <v>220</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
     </row>
     <row r="4" spans="1:11">
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="33" t="s">
         <v>221</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="33" t="s">
         <v>222</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
     </row>
     <row r="8" spans="1:11">
       <c r="B8" s="17"/>

</xml_diff>

<commit_message>
Change SBOM in template file
</commit_message>
<xml_diff>
--- a/src/main/resources/template/OssCheckList.xlsx
+++ b/src/main/resources/template/OssCheckList.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11018"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\FOSSLight\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/min/Min/ui_2.0/fosslight/src/main/resources/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965A27A1-FAB3-D642-85DC-E5BE9F04A8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34836" yWindow="3912" windowWidth="32376" windowHeight="14868"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17320" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3rd Party Info" sheetId="10" r:id="rId1"/>
     <sheet name="3rd Party" sheetId="1" r:id="rId2"/>
-    <sheet name="3rd Party - BOM" sheetId="7" r:id="rId3"/>
+    <sheet name="3rd Party - SBOM" sheetId="7" r:id="rId3"/>
     <sheet name="3rd Party - Security" sheetId="8" r:id="rId4"/>
     <sheet name=".Data" sheetId="6" state="hidden" r:id="rId5"/>
   </sheets>
@@ -22,17 +23,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'.Data'!$A$1:$A$163</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -845,7 +835,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="34">
     <font>
       <sz val="11"/>
@@ -1793,25 +1783,11 @@
     <cellStyle name="좋음" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="출력" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="표준 2" xfId="42"/>
-    <cellStyle name="標準_07FBDP_メニュー画面仕様書_Ver0.01.00" xfId="43"/>
+    <cellStyle name="표준 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="標準_07FBDP_メニュー画面仕様書_Ver0.01.00" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
     <cellStyle name="하이퍼링크" xfId="44" builtinId="8"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -2101,19 +2077,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="37.3984375" customWidth="1"/>
-    <col min="2" max="2" width="45.69921875" style="26" customWidth="1"/>
-    <col min="3" max="3" width="120.59765625" style="27" customWidth="1"/>
-    <col min="5" max="5" width="20.09765625" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" style="26" customWidth="1"/>
+    <col min="3" max="3" width="120.6640625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2195,18 +2171,18 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="B3"/>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="B3" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Calibri"&amp;12&amp;K000000LGE Internal Use Only&amp;1#</oddHeader>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;K000000 LGE Internal Use Only&amp;1#_x000D_</oddHeader>
   </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P500"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2214,20 +2190,20 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="5.59765625" customWidth="1"/>
-    <col min="2" max="2" width="30.59765625" customWidth="1"/>
-    <col min="3" max="3" width="20.59765625" customWidth="1"/>
-    <col min="4" max="4" width="10.59765625" style="11" customWidth="1"/>
-    <col min="5" max="7" width="20.59765625" customWidth="1"/>
-    <col min="8" max="9" width="30.59765625" customWidth="1"/>
-    <col min="10" max="10" width="20.59765625" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="11" customWidth="1"/>
+    <col min="5" max="7" width="20.6640625" customWidth="1"/>
+    <col min="8" max="9" width="30.6640625" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" customWidth="1"/>
     <col min="11" max="11" width="11.5" customWidth="1"/>
-    <col min="12" max="12" width="30.59765625" customWidth="1"/>
-    <col min="13" max="14" width="10.59765625" customWidth="1"/>
-    <col min="15" max="15" width="20.59765625" customWidth="1"/>
-    <col min="16" max="16" width="40.59765625" customWidth="1"/>
+    <col min="12" max="12" width="30.6640625" customWidth="1"/>
+    <col min="13" max="14" width="10.6640625" customWidth="1"/>
+    <col min="15" max="15" width="20.6640625" customWidth="1"/>
+    <col min="16" max="16" width="40.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -11305,17 +11281,20 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" sqref="E1:E2 K1:K2"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="K3:K1048576">
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="E1:E2 K1:K2" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="K3:K1048576" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Exclude"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;K000000 LGE Internal Use Only&amp;1#_x000D_</oddHeader>
+  </headerFooter>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>'.Data'!$A$2:$A$177</xm:f>
           </x14:formula1>
@@ -11328,23 +11307,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N499"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:N1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="5.59765625" customWidth="1"/>
-    <col min="2" max="2" width="20.59765625" customWidth="1"/>
-    <col min="3" max="3" width="10.59765625" style="11" customWidth="1"/>
-    <col min="4" max="6" width="20.59765625" customWidth="1"/>
-    <col min="7" max="8" width="30.59765625" customWidth="1"/>
-    <col min="9" max="9" width="10.59765625" customWidth="1"/>
-    <col min="10" max="13" width="13.09765625" customWidth="1"/>
-    <col min="14" max="14" width="18.19921875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" style="11" customWidth="1"/>
+    <col min="4" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="8" width="30.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="10" max="13" width="13.1640625" customWidth="1"/>
+    <col min="14" max="14" width="18.1640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -18870,29 +18849,32 @@
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;K000000 LGE Internal Use Only&amp;1#_x000D_</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:K1001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="3.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.09765625" customWidth="1"/>
-    <col min="6" max="6" width="18.69921875" customWidth="1"/>
-    <col min="7" max="7" width="23.3984375" customWidth="1"/>
-    <col min="8" max="8" width="25.09765625" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="23.33203125" customWidth="1"/>
+    <col min="8" max="8" width="25.1640625" customWidth="1"/>
     <col min="9" max="9" width="41" customWidth="1"/>
-    <col min="10" max="10" width="40.69921875" customWidth="1"/>
+    <col min="10" max="10" width="40.6640625" customWidth="1"/>
     <col min="11" max="11" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -25969,21 +25951,24 @@
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G10:G1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G10:G1048576" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Unresolved, Fixed, Will be fixed (MR), Will be fixed (External Dependency), Deferred (Not Available), Won't fix (Mitigation), Won't fix (Drop)"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;K000000 LGE Internal Use Only&amp;1#_x000D_</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:A177"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="67" style="2" customWidth="1"/>
     <col min="2" max="16384" width="9" style="2"/>
@@ -25994,812 +25979,812 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" ht="18">
       <c r="A2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" ht="18">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" ht="18">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" ht="18">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" ht="18">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" ht="18">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" ht="18">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" ht="18">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" ht="18">
       <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" ht="18">
       <c r="A11" s="3" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" ht="18">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" ht="18">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" ht="18">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" ht="18">
       <c r="A15" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" ht="18">
       <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" ht="18">
       <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" ht="18">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" ht="18">
       <c r="A19" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" ht="18">
       <c r="A20" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" ht="18">
       <c r="A21" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" ht="18">
       <c r="A22" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" ht="18">
       <c r="A23" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" ht="18">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" ht="18">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" ht="18">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" ht="18">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" ht="18">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" ht="18">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" ht="18">
       <c r="A30" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" ht="18">
       <c r="A31" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" ht="18">
       <c r="A32" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" ht="18">
       <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" ht="18">
       <c r="A34" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="35" spans="1:1">
+    <row r="35" spans="1:1" ht="18">
       <c r="A35" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:1">
+    <row r="36" spans="1:1" ht="18">
       <c r="A36" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:1">
+    <row r="37" spans="1:1" ht="18">
       <c r="A37" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:1">
+    <row r="38" spans="1:1" ht="18">
       <c r="A38" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:1">
+    <row r="39" spans="1:1" ht="18">
       <c r="A39" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:1">
+    <row r="40" spans="1:1" ht="18">
       <c r="A40" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:1">
+    <row r="41" spans="1:1" ht="18">
       <c r="A41" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:1">
+    <row r="42" spans="1:1" ht="18">
       <c r="A42" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:1">
+    <row r="43" spans="1:1" ht="18">
       <c r="A43" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="44" spans="1:1">
+    <row r="44" spans="1:1" ht="18">
       <c r="A44" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="45" spans="1:1">
+    <row r="45" spans="1:1" ht="18">
       <c r="A45" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:1">
+    <row r="46" spans="1:1" ht="18">
       <c r="A46" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:1">
+    <row r="47" spans="1:1" ht="18">
       <c r="A47" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:1">
+    <row r="48" spans="1:1" ht="18">
       <c r="A48" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:1">
+    <row r="49" spans="1:1" ht="18">
       <c r="A49" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:1">
+    <row r="50" spans="1:1" ht="18">
       <c r="A50" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:1">
+    <row r="51" spans="1:1" ht="18">
       <c r="A51" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="52" spans="1:1">
+    <row r="52" spans="1:1" ht="18">
       <c r="A52" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="53" spans="1:1">
+    <row r="53" spans="1:1" ht="18">
       <c r="A53" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="54" spans="1:1">
+    <row r="54" spans="1:1" ht="18">
       <c r="A54" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="1:1">
+    <row r="55" spans="1:1" ht="18">
       <c r="A55" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="56" spans="1:1">
+    <row r="56" spans="1:1" ht="18">
       <c r="A56" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="1:1">
+    <row r="57" spans="1:1" ht="18">
       <c r="A57" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="58" spans="1:1">
+    <row r="58" spans="1:1" ht="18">
       <c r="A58" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="1:1">
+    <row r="59" spans="1:1" ht="18">
       <c r="A59" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="60" spans="1:1">
+    <row r="60" spans="1:1" ht="18">
       <c r="A60" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="61" spans="1:1">
+    <row r="61" spans="1:1" ht="18">
       <c r="A61" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:1">
+    <row r="62" spans="1:1" ht="18">
       <c r="A62" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:1">
+    <row r="63" spans="1:1" ht="18">
       <c r="A63" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="64" spans="1:1">
+    <row r="64" spans="1:1" ht="18">
       <c r="A64" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:1" ht="18">
       <c r="A65" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:1" ht="18">
       <c r="A66" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="67" spans="1:1">
+    <row r="67" spans="1:1" ht="18">
       <c r="A67" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:1" ht="18">
       <c r="A68" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:1" ht="18">
       <c r="A69" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:1">
+    <row r="70" spans="1:1" ht="18">
       <c r="A70" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:1" ht="18">
       <c r="A71" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="1:1">
+    <row r="72" spans="1:1" ht="18">
       <c r="A72" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="1:1">
+    <row r="73" spans="1:1" ht="18">
       <c r="A73" s="3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="74" spans="1:1">
+    <row r="74" spans="1:1" ht="18">
       <c r="A74" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="1:1">
+    <row r="75" spans="1:1" ht="18">
       <c r="A75" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="76" spans="1:1">
+    <row r="76" spans="1:1" ht="18">
       <c r="A76" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:1">
+    <row r="77" spans="1:1" ht="18">
       <c r="A77" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="78" spans="1:1">
+    <row r="78" spans="1:1" ht="18">
       <c r="A78" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="79" spans="1:1">
+    <row r="79" spans="1:1" ht="18">
       <c r="A79" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:1">
+    <row r="80" spans="1:1" ht="18">
       <c r="A80" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="81" spans="1:1">
+    <row r="81" spans="1:1" ht="18">
       <c r="A81" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="82" spans="1:1">
+    <row r="82" spans="1:1" ht="18">
       <c r="A82" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="83" spans="1:1">
+    <row r="83" spans="1:1" ht="18">
       <c r="A83" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="84" spans="1:1">
+    <row r="84" spans="1:1" ht="18">
       <c r="A84" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:1">
+    <row r="85" spans="1:1" ht="18">
       <c r="A85" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="86" spans="1:1">
+    <row r="86" spans="1:1" ht="18">
       <c r="A86" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="87" spans="1:1">
+    <row r="87" spans="1:1" ht="18">
       <c r="A87" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="88" spans="1:1">
+    <row r="88" spans="1:1" ht="18">
       <c r="A88" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="89" spans="1:1">
+    <row r="89" spans="1:1" ht="18">
       <c r="A89" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="90" spans="1:1">
+    <row r="90" spans="1:1" ht="18">
       <c r="A90" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="91" spans="1:1">
+    <row r="91" spans="1:1" ht="18">
       <c r="A91" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="92" spans="1:1">
+    <row r="92" spans="1:1" ht="18">
       <c r="A92" s="3" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="93" spans="1:1">
+    <row r="93" spans="1:1" ht="18">
       <c r="A93" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="94" spans="1:1">
+    <row r="94" spans="1:1" ht="18">
       <c r="A94" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="95" spans="1:1">
+    <row r="95" spans="1:1" ht="18">
       <c r="A95" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="96" spans="1:1">
+    <row r="96" spans="1:1" ht="18">
       <c r="A96" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" ht="18">
       <c r="A97" s="3" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" ht="18">
       <c r="A98" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" ht="18">
       <c r="A99" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" ht="18">
       <c r="A100" s="3" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" ht="18">
       <c r="A101" s="3" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" ht="18">
       <c r="A102" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" ht="18">
       <c r="A103" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" ht="18">
       <c r="A104" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" ht="18">
       <c r="A105" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" ht="18">
       <c r="A106" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" ht="18">
       <c r="A107" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" ht="18">
       <c r="A108" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" ht="18">
       <c r="A109" s="3" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" ht="18">
       <c r="A110" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:1" ht="18">
       <c r="A111" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:1" ht="18">
       <c r="A112" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="113" spans="1:1">
+    <row r="113" spans="1:1" ht="18">
       <c r="A113" s="3" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="114" spans="1:1">
+    <row r="114" spans="1:1" ht="18">
       <c r="A114" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="115" spans="1:1">
+    <row r="115" spans="1:1" ht="18">
       <c r="A115" s="3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="116" spans="1:1">
+    <row r="116" spans="1:1" ht="18">
       <c r="A116" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="117" spans="1:1">
+    <row r="117" spans="1:1" ht="18">
       <c r="A117" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="118" spans="1:1">
+    <row r="118" spans="1:1" ht="18">
       <c r="A118" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="119" spans="1:1">
+    <row r="119" spans="1:1" ht="18">
       <c r="A119" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="120" spans="1:1">
+    <row r="120" spans="1:1" ht="18">
       <c r="A120" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="121" spans="1:1">
+    <row r="121" spans="1:1" ht="18">
       <c r="A121" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="122" spans="1:1">
+    <row r="122" spans="1:1" ht="18">
       <c r="A122" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="123" spans="1:1">
+    <row r="123" spans="1:1" ht="18">
       <c r="A123" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="124" spans="1:1">
+    <row r="124" spans="1:1" ht="18">
       <c r="A124" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="125" spans="1:1">
+    <row r="125" spans="1:1" ht="18">
       <c r="A125" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="126" spans="1:1">
+    <row r="126" spans="1:1" ht="18">
       <c r="A126" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="127" spans="1:1">
+    <row r="127" spans="1:1" ht="18">
       <c r="A127" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="128" spans="1:1">
+    <row r="128" spans="1:1" ht="18">
       <c r="A128" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="129" spans="1:1">
+    <row r="129" spans="1:1" ht="18">
       <c r="A129" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="130" spans="1:1">
+    <row r="130" spans="1:1" ht="18">
       <c r="A130" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="131" spans="1:1">
+    <row r="131" spans="1:1" ht="18">
       <c r="A131" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="132" spans="1:1">
+    <row r="132" spans="1:1" ht="18">
       <c r="A132" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="133" spans="1:1">
+    <row r="133" spans="1:1" ht="18">
       <c r="A133" s="3" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="134" spans="1:1">
+    <row r="134" spans="1:1" ht="18">
       <c r="A134" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="135" spans="1:1">
+    <row r="135" spans="1:1" ht="18">
       <c r="A135" s="3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="136" spans="1:1">
+    <row r="136" spans="1:1" ht="18">
       <c r="A136" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="137" spans="1:1">
+    <row r="137" spans="1:1" ht="18">
       <c r="A137" s="3" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="138" spans="1:1">
+    <row r="138" spans="1:1" ht="18">
       <c r="A138" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="139" spans="1:1">
+    <row r="139" spans="1:1" ht="18">
       <c r="A139" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="140" spans="1:1">
+    <row r="140" spans="1:1" ht="18">
       <c r="A140" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="141" spans="1:1">
+    <row r="141" spans="1:1" ht="18">
       <c r="A141" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="142" spans="1:1">
+    <row r="142" spans="1:1" ht="18">
       <c r="A142" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="143" spans="1:1">
+    <row r="143" spans="1:1" ht="18">
       <c r="A143" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="144" spans="1:1">
+    <row r="144" spans="1:1" ht="18">
       <c r="A144" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="145" spans="1:1">
+    <row r="145" spans="1:1" ht="18">
       <c r="A145" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="146" spans="1:1">
+    <row r="146" spans="1:1" ht="18">
       <c r="A146" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="147" spans="1:1">
+    <row r="147" spans="1:1" ht="18">
       <c r="A147" s="3" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="148" spans="1:1">
+    <row r="148" spans="1:1" ht="18">
       <c r="A148" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="149" spans="1:1">
+    <row r="149" spans="1:1" ht="18">
       <c r="A149" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="150" spans="1:1">
+    <row r="150" spans="1:1" ht="18">
       <c r="A150" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="151" spans="1:1">
+    <row r="151" spans="1:1" ht="18">
       <c r="A151" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="152" spans="1:1">
+    <row r="152" spans="1:1" ht="18">
       <c r="A152" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="153" spans="1:1">
+    <row r="153" spans="1:1" ht="18">
       <c r="A153" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="154" spans="1:1">
+    <row r="154" spans="1:1" ht="18">
       <c r="A154" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="155" spans="1:1">
+    <row r="155" spans="1:1" ht="18">
       <c r="A155" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="156" spans="1:1">
+    <row r="156" spans="1:1" ht="18">
       <c r="A156" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="157" spans="1:1">
+    <row r="157" spans="1:1" ht="18">
       <c r="A157" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="158" spans="1:1">
+    <row r="158" spans="1:1" ht="18">
       <c r="A158" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="159" spans="1:1">
+    <row r="159" spans="1:1" ht="18">
       <c r="A159" s="3" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="160" spans="1:1">
+    <row r="160" spans="1:1" ht="18">
       <c r="A160" s="3" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="161" spans="1:1">
+    <row r="161" spans="1:1" ht="18">
       <c r="A161" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="162" spans="1:1">
+    <row r="162" spans="1:1" ht="18">
       <c r="A162" s="3" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="163" spans="1:1">
+    <row r="163" spans="1:1" ht="18">
       <c r="A163" s="3" t="s">
         <v>177</v>
       </c>
@@ -26875,12 +26860,15 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A163">
-    <sortState ref="A31:A191">
+  <autoFilter ref="A1:A163" xr:uid="{00000000-0009-0000-0000-000004000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A31:A191">
       <sortCondition ref="A31:A191"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Aptos"&amp;12&amp;K000000 LGE Internal Use Only&amp;1#_x000D_</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>